<commit_message>
add pics and listings
</commit_message>
<xml_diff>
--- a/Lab 7/PHYS351lab7.xlsx
+++ b/Lab 7/PHYS351lab7.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="240" windowWidth="25360" windowHeight="14360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2040" yWindow="0" windowWidth="25380" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="question 2" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>V_in</t>
   </si>
@@ -36,6 +36,18 @@
   </si>
   <si>
     <t>*note this is a rail don't include in graph</t>
+  </si>
+  <si>
+    <t>vin-vmbed</t>
+  </si>
+  <si>
+    <t>p-error</t>
+  </si>
+  <si>
+    <t>vmbed-vout</t>
+  </si>
+  <si>
+    <t>perror</t>
   </si>
 </sst>
 </file>
@@ -92,8 +104,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -101,14 +123,657 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Percent Error Vs. Voltage In</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'question 2'!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.522</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.769</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.322</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.532</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.715</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.052</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.244</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.878</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.068</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.078</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.979</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.044</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'question 2'!$D$2:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.0347826086956522</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0134099616858238</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0208062418725618</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000952380952381059</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0136157337367625</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00587467362924275</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00233236151603499</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.00389863547758285</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0650623885918003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.00588235294117652</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.000694927032661648</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.000325945241199442</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.00278293135435982</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.00151591712986362</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.00558475689881731</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2124434200"/>
+        <c:axId val="-2125416200"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2124434200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:t>Voltage</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                  <a:t> In</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="2000"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2125416200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2125416200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:t>Percent Error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2124434200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Requested output vs. Percent Error</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'question 3'!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'question 3'!$D$2:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.044</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0133333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00899999999999989</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.00228571428571429</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.000888888888888791</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.000399999999999956</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.00181818181818178</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.00233333333333337</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.00153846153846151</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.00899999999999989</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.00233333333333337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2088691032"/>
+        <c:axId val="-2088688072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2088691032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:t>Requested output voltage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2088688072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2088688072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:t>Percent Error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2088691032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>142240</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>111760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -433,160 +1098,304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
+        <v>0.23</v>
+      </c>
+      <c r="B2">
+        <v>0.222</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C16" si="0">ABS(A2-B2)</f>
+        <v>8.0000000000000071E-3</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D16" si="1">C2/A2</f>
+        <v>3.4782608695652202E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="B3">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000062E-3</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="1"/>
+        <v>1.3409961685823766E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="B4">
+        <v>0.753</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>1.6000000000000014E-2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>2.0806241872561786E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>1.05</v>
+      </c>
+      <c r="B5">
+        <v>1.0489999999999999</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>1.0000000000001119E-3</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>9.5238095238105896E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>1.3220000000000001</v>
+      </c>
+      <c r="B6">
+        <v>1.34</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1.8000000000000016E-2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1.3615733736762493E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>1.532</v>
+      </c>
+      <c r="B7">
+        <v>1.5409999999999999</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>8.999999999999897E-3</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>5.8746736292427529E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>1.7150000000000001</v>
+      </c>
+      <c r="B8">
+        <v>1.7190000000000001</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>2.3323615160349876E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>2.052</v>
+      </c>
+      <c r="B9">
+        <v>2.06</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000071E-3</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>3.8986354775828493E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>2.2440000000000002</v>
+      </c>
+      <c r="B10">
+        <v>2.39</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.14599999999999991</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>6.5062388591800316E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="B11">
+        <v>2.5649999999999999</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>1.5000000000000124E-2</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>5.8823529411765199E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>2.8780000000000001</v>
+      </c>
+      <c r="B12">
+        <v>2.8759999999999999</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>2.0000000000002238E-3</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>6.9492703266164826E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>3.0680000000000001</v>
+      </c>
+      <c r="B13">
+        <v>3.069</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999988987E-4</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>3.2594524119944259E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>1.0780000000000001</v>
+      </c>
+      <c r="B14">
+        <v>1.081</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>2.9999999999998916E-3</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>2.7829313543598251E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>1.9790000000000001</v>
+      </c>
+      <c r="B15">
+        <v>1.976</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>3.0000000000001137E-3</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>1.5159171298636249E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>3.044</v>
+      </c>
+      <c r="B16">
+        <v>3.0609999999999999</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>1.6999999999999904E-2</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>5.5847568988173137E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="B2">
+      <c r="B19">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>0.23</v>
-      </c>
-      <c r="B3">
-        <v>0.222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>0.52200000000000002</v>
-      </c>
-      <c r="B4">
-        <v>0.52900000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>0.76900000000000002</v>
-      </c>
-      <c r="B5">
-        <v>0.753</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>1.05</v>
-      </c>
-      <c r="B6">
-        <v>1.0489999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>1.3220000000000001</v>
-      </c>
-      <c r="B7">
-        <v>1.34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>1.532</v>
-      </c>
-      <c r="B8">
-        <v>1.5409999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>1.7150000000000001</v>
-      </c>
-      <c r="B9">
-        <v>1.7190000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>2.052</v>
-      </c>
-      <c r="B10">
-        <v>2.06</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>2.2440000000000002</v>
-      </c>
-      <c r="B11">
-        <v>2.39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="B12">
-        <v>2.5649999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
-        <v>2.8780000000000001</v>
-      </c>
-      <c r="B13">
-        <v>2.8759999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
-        <v>3.0680000000000001</v>
-      </c>
-      <c r="B14">
-        <v>3.069</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
+      <c r="C19">
+        <f>ABS(A19-B19)</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D19">
+        <f>C19/A19</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="B15">
+      <c r="B20">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
-        <v>1.0780000000000001</v>
-      </c>
-      <c r="B16">
-        <v>1.081</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
-        <v>1.9790000000000001</v>
-      </c>
-      <c r="B17">
-        <v>1.976</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
-        <v>3.044</v>
-      </c>
-      <c r="B18">
-        <v>3.0609999999999999</v>
+      <c r="C20">
+        <f>ABS(A20-B20)</f>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D20">
+        <f>C20/A20</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -597,180 +1406,335 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
         <v>2.8000000000000001E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2">
+        <f>ABS(A2-B2)</f>
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="D2" t="e">
+        <f>C2/A2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>0.25</v>
       </c>
       <c r="B3">
         <v>0.27500000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="C3">
+        <f t="shared" ref="C3:C19" si="0">ABS(A3-B3)</f>
+        <v>2.5000000000000022E-2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D19" si="1">C3/A3</f>
+        <v>0.10000000000000009</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>0.5</v>
       </c>
       <c r="B4">
         <v>0.52200000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>2.200000000000002E-2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>4.4000000000000039E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>0.75</v>
       </c>
       <c r="B5">
         <v>0.76</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>1.3333333333333345E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6">
         <v>1.0089999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>8.999999999999897E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>8.999999999999897E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>1.25</v>
       </c>
       <c r="B7">
         <v>1.2549999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>3.9999999999999151E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>1.5</v>
       </c>
       <c r="B8">
         <v>1.506</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>6.0000000000000053E-3</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000036E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>1.75</v>
       </c>
       <c r="B9">
         <v>1.754</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>2.2857142857142876E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10">
         <v>2.004</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>2.0000000000000018E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>2.25</v>
       </c>
       <c r="B11">
         <v>2.2519999999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>1.9999999999997797E-3</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>8.8888888888879103E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>2.5</v>
       </c>
       <c r="B12">
         <v>2.5009999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>9.9999999999988987E-4</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>3.9999999999995595E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>2.75</v>
       </c>
       <c r="B13">
         <v>2.7549999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>1.8181818181817794E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>3</v>
       </c>
       <c r="B14">
         <v>3.0070000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>7.0000000000001172E-3</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>2.3333333333333726E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>3.25</v>
       </c>
       <c r="B15">
         <v>3.2549999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>1.5384615384615057E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="D16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>1.0089999999999999</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>8.999999999999897E-3</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>8.999999999999897E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>2.004</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>2.0000000000000018E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>3.0070000000000001</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>7.0000000000001172E-3</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>2.3333333333333726E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
         <v>5</v>
       </c>
-      <c r="B16">
+      <c r="B25">
         <v>3.3969999999999998</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C25">
+        <f>ABS(A25-B25)</f>
+        <v>1.6030000000000002</v>
+      </c>
+      <c r="E25" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18">
-        <v>1.0089999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19">
-        <v>2.004</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20">
-        <v>3.0070000000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>